<commit_message>
Cleaned up species excel
</commit_message>
<xml_diff>
--- a/map_data/voedselbos_species.xlsx
+++ b/map_data/voedselbos_species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\map_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4833DC01-7481-4394-829A-E75B8D154C0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09033A7-9EB8-437E-BA0A-DF9D3AE1CB34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="-615" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="423">
   <si>
     <t>Hovenia dulcis</t>
   </si>
@@ -393,9 +393,6 @@
     <t>Olijfwilg</t>
   </si>
   <si>
-    <t>5 </t>
-  </si>
-  <si>
     <t>Prunus avium, halfstam</t>
   </si>
   <si>
@@ -538,9 +535,6 @@
   </si>
   <si>
     <t>Steeneik</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Crataegus calpodendron</t>
@@ -1009,9 +1003,6 @@
     <t>R. typhina</t>
   </si>
   <si>
-    <t>R.phoenicolasius</t>
-  </si>
-  <si>
     <t>S. argentea</t>
   </si>
   <si>
@@ -1307,6 +1298,9 @@
   </si>
   <si>
     <t>Shallon (appeltjesblad)</t>
+  </si>
+  <si>
+    <t>R. phoenicolasius</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1662,7 @@
   <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,50 +1677,50 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -1740,7 +1734,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1760,7 +1754,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1769,7 +1763,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1783,7 +1777,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
@@ -1800,13 +1794,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -1817,16 +1811,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1835,18 +1829,18 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E9">
         <v>0.25</v>
@@ -1857,16 +1851,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B10" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D10" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1891,13 +1885,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E12">
         <v>2.5</v>
@@ -1908,13 +1902,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E13">
         <v>2.5</v>
@@ -1923,18 +1917,18 @@
         <v>2.5</v>
       </c>
       <c r="G13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="s">
         <v>181</v>
-      </c>
-      <c r="C14" t="s">
-        <v>183</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1943,18 +1937,18 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1965,13 +1959,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E16">
         <v>12</v>
@@ -1982,24 +1976,24 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -2010,13 +2004,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -2025,12 +2019,12 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -2050,10 +2044,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C21" t="s">
         <v>77</v>
@@ -2067,13 +2061,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" t="s">
         <v>178</v>
-      </c>
-      <c r="C22" t="s">
-        <v>180</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -2082,12 +2076,12 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
@@ -2104,16 +2098,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D24" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -2122,12 +2116,12 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
@@ -2136,7 +2130,7 @@
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2150,16 +2144,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D26" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E26">
         <v>1.5</v>
@@ -2168,21 +2162,21 @@
         <v>1.5</v>
       </c>
       <c r="G26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" t="s">
         <v>186</v>
       </c>
-      <c r="C27" t="s">
-        <v>188</v>
-      </c>
       <c r="D27" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2191,12 +2185,12 @@
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
@@ -2205,7 +2199,7 @@
         <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E28">
         <v>8</v>
@@ -2219,13 +2213,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -2234,21 +2228,21 @@
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" t="s">
         <v>241</v>
       </c>
-      <c r="C30" t="s">
-        <v>243</v>
-      </c>
       <c r="D30" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E30">
         <v>6</v>
@@ -2257,12 +2251,12 @@
         <v>6</v>
       </c>
       <c r="G30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
@@ -2271,7 +2265,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -2282,7 +2276,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B32" t="s">
         <v>104</v>
@@ -2291,7 +2285,7 @@
         <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -2302,16 +2296,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C33" t="s">
         <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -2322,7 +2316,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B34" t="s">
         <v>96</v>
@@ -2331,7 +2325,7 @@
         <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E34">
         <v>6</v>
@@ -2345,7 +2339,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
@@ -2354,7 +2348,7 @@
         <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E35">
         <v>6</v>
@@ -2365,7 +2359,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s">
         <v>99</v>
@@ -2374,7 +2368,7 @@
         <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E36">
         <v>9</v>
@@ -2388,16 +2382,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C37" t="s">
         <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E37">
         <v>6</v>
@@ -2406,12 +2400,12 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B38" t="s">
         <v>101</v>
@@ -2420,7 +2414,7 @@
         <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E38">
         <v>7</v>
@@ -2431,7 +2425,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B39" t="s">
         <v>102</v>
@@ -2440,7 +2434,7 @@
         <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -2451,7 +2445,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B40" t="s">
         <v>105</v>
@@ -2460,7 +2454,7 @@
         <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -2471,13 +2465,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -2486,12 +2480,12 @@
         <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -2508,7 +2502,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -2525,13 +2519,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B44" t="s">
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -2542,7 +2536,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B45" t="s">
         <v>115</v>
@@ -2550,7 +2544,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B46" t="s">
         <v>94</v>
@@ -2567,13 +2561,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -2582,18 +2576,18 @@
         <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -2602,12 +2596,12 @@
         <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B49" t="s">
         <v>113</v>
@@ -2624,13 +2618,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C50" t="s">
         <v>232</v>
-      </c>
-      <c r="C50" t="s">
-        <v>234</v>
       </c>
       <c r="E50">
         <v>3</v>
@@ -2639,12 +2633,12 @@
         <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B51" t="s">
         <v>107</v>
@@ -2653,7 +2647,7 @@
         <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E51">
         <v>3</v>
@@ -2667,7 +2661,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B52" t="s">
         <v>118</v>
@@ -2675,8 +2669,8 @@
       <c r="C52" t="s">
         <v>119</v>
       </c>
-      <c r="E52" t="s">
-        <v>120</v>
+      <c r="E52">
+        <v>5</v>
       </c>
       <c r="F52">
         <v>5</v>
@@ -2684,13 +2678,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C53" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E53">
         <v>6</v>
@@ -2701,13 +2695,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C54" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -2716,18 +2710,18 @@
         <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
         <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E55">
         <v>6</v>
@@ -2741,13 +2735,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E56">
         <v>2.5</v>
@@ -2758,13 +2752,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B57" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" t="s">
         <v>193</v>
-      </c>
-      <c r="C57" t="s">
-        <v>195</v>
       </c>
       <c r="E57">
         <v>2.5</v>
@@ -2773,32 +2767,32 @@
         <v>2</v>
       </c>
       <c r="G57" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C58" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B59" t="s">
         <v>90</v>
       </c>
       <c r="C59" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D59" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E59">
         <v>1.5</v>
@@ -2809,13 +2803,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B60" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C60" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E60">
         <v>10</v>
@@ -2826,16 +2820,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D61" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E61">
         <v>20</v>
@@ -2846,7 +2840,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B62" t="s">
         <v>78</v>
@@ -2863,7 +2857,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B63" t="s">
         <v>38</v>
@@ -2897,13 +2891,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B65" t="s">
+        <v>216</v>
+      </c>
+      <c r="C65" t="s">
         <v>218</v>
-      </c>
-      <c r="C65" t="s">
-        <v>220</v>
       </c>
       <c r="E65">
         <v>6</v>
@@ -2912,18 +2906,18 @@
         <v>5</v>
       </c>
       <c r="G65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E66">
         <v>10</v>
@@ -2934,13 +2928,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B67" t="s">
+        <v>196</v>
+      </c>
+      <c r="C67" t="s">
         <v>198</v>
-      </c>
-      <c r="C67" t="s">
-        <v>200</v>
       </c>
       <c r="E67">
         <v>2.5</v>
@@ -2949,18 +2943,18 @@
         <v>2.5</v>
       </c>
       <c r="G67" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B68" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C68" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E68">
         <v>10</v>
@@ -2974,13 +2968,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B69" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C69" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E69">
         <v>10</v>
@@ -2991,7 +2985,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B70" t="s">
         <v>110</v>
@@ -3011,13 +3005,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E71">
         <v>15</v>
@@ -3026,18 +3020,18 @@
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E72">
         <v>8</v>
@@ -3046,18 +3040,18 @@
         <v>12</v>
       </c>
       <c r="G72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E73">
         <v>15</v>
@@ -3066,32 +3060,32 @@
         <v>10</v>
       </c>
       <c r="G73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>363</v>
+      </c>
+      <c r="B74" t="s">
         <v>366</v>
       </c>
-      <c r="B74" t="s">
-        <v>369</v>
-      </c>
       <c r="C74" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D74" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E75">
         <v>6</v>
@@ -3102,7 +3096,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B76" t="s">
         <v>40</v>
@@ -3122,16 +3116,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B77" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" t="s">
         <v>171</v>
       </c>
-      <c r="C77" t="s">
-        <v>173</v>
-      </c>
       <c r="D77" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E77">
         <v>20</v>
@@ -3140,35 +3134,35 @@
         <v>15</v>
       </c>
       <c r="G77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D79" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E79">
         <v>6</v>
@@ -3177,18 +3171,18 @@
         <v>4</v>
       </c>
       <c r="G79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -3197,18 +3191,18 @@
         <v>4</v>
       </c>
       <c r="G80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3217,32 +3211,32 @@
         <v>3</v>
       </c>
       <c r="G81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B82" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C82" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D82" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B83" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" t="s">
         <v>131</v>
-      </c>
-      <c r="C83" t="s">
-        <v>132</v>
       </c>
       <c r="E83">
         <v>7</v>
@@ -3253,13 +3247,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E84">
         <v>10</v>
@@ -3273,30 +3267,24 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B85" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" t="s">
         <v>167</v>
-      </c>
-      <c r="C85" t="s">
-        <v>168</v>
-      </c>
-      <c r="E85" t="s">
-        <v>169</v>
-      </c>
-      <c r="F85" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B86" t="s">
         <v>43</v>
       </c>
       <c r="C86" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E86">
         <v>1.5</v>
@@ -3310,7 +3298,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B87" t="s">
         <v>45</v>
@@ -3327,7 +3315,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B88" t="s">
         <v>91</v>
@@ -3347,7 +3335,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B89" t="s">
         <v>47</v>
@@ -3364,7 +3352,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B90" t="s">
         <v>49</v>
@@ -3373,7 +3361,7 @@
         <v>51</v>
       </c>
       <c r="D90" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -3387,13 +3375,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B91" t="s">
+        <v>199</v>
+      </c>
+      <c r="C91" t="s">
         <v>201</v>
-      </c>
-      <c r="C91" t="s">
-        <v>203</v>
       </c>
       <c r="E91">
         <v>1.25</v>
@@ -3402,12 +3390,12 @@
         <v>1.25</v>
       </c>
       <c r="G91" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
@@ -3427,13 +3415,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B93" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C93" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E93">
         <v>2</v>
@@ -3442,12 +3430,12 @@
         <v>1.5</v>
       </c>
       <c r="G93" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
@@ -3461,7 +3449,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
@@ -3478,16 +3466,16 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B96" t="s">
         <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D96" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E96">
         <v>0.5</v>
@@ -3498,7 +3486,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>325</v>
+        <v>422</v>
       </c>
       <c r="B97" t="s">
         <v>57</v>
@@ -3507,7 +3495,7 @@
         <v>58</v>
       </c>
       <c r="D97" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -3518,13 +3506,13 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B98" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" t="s">
         <v>204</v>
-      </c>
-      <c r="C98" t="s">
-        <v>206</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -3533,23 +3521,23 @@
         <v>3</v>
       </c>
       <c r="G98" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B99" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C99" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B100" t="s">
         <v>116</v>
@@ -3558,7 +3546,7 @@
         <v>61</v>
       </c>
       <c r="D100" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E100">
         <v>3</v>
@@ -3572,7 +3560,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B101" t="s">
         <v>59</v>
@@ -3592,7 +3580,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B102" t="s">
         <v>62</v>
@@ -3609,7 +3597,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B103" t="s">
         <v>64</v>
@@ -3629,7 +3617,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B104" t="s">
         <v>67</v>
@@ -3646,13 +3634,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B105" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C105" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E105">
         <v>20</v>
@@ -3661,12 +3649,12 @@
         <v>8</v>
       </c>
       <c r="G105" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B106" t="s">
         <v>3</v>
@@ -3675,7 +3663,7 @@
         <v>4</v>
       </c>
       <c r="D106" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E106">
         <v>20</v>
@@ -3686,7 +3674,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B107" t="s">
         <v>69</v>
@@ -3703,13 +3691,13 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B108" t="s">
+        <v>207</v>
+      </c>
+      <c r="C108" t="s">
         <v>209</v>
-      </c>
-      <c r="C108" t="s">
-        <v>211</v>
       </c>
       <c r="E108">
         <v>3</v>
@@ -3718,18 +3706,18 @@
         <v>3</v>
       </c>
       <c r="G108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B109" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E109">
         <v>3</v>
@@ -3740,13 +3728,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E110">
         <v>3</v>
@@ -3757,7 +3745,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -3766,7 +3754,7 @@
         <v>7</v>
       </c>
       <c r="D111" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E111">
         <v>20</v>
@@ -3777,7 +3765,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B112" t="s">
         <v>80</v>
@@ -3794,7 +3782,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B113" t="s">
         <v>85</v>
@@ -3814,16 +3802,16 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>382</v>
+      </c>
+      <c r="B114" t="s">
+        <v>172</v>
+      </c>
+      <c r="C114" t="s">
         <v>385</v>
       </c>
-      <c r="B114" t="s">
-        <v>174</v>
-      </c>
-      <c r="C114" t="s">
-        <v>388</v>
-      </c>
       <c r="D114" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E114">
         <v>0.5</v>
@@ -3834,16 +3822,16 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>381</v>
+      </c>
+      <c r="B115" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" t="s">
         <v>384</v>
       </c>
-      <c r="B115" t="s">
-        <v>175</v>
-      </c>
-      <c r="C115" t="s">
-        <v>387</v>
-      </c>
       <c r="D115" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E115">
         <v>0.2</v>
@@ -3854,7 +3842,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B116" t="s">
         <v>71</v>
@@ -3863,7 +3851,7 @@
         <v>72</v>
       </c>
       <c r="D116" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E116">
         <v>2</v>
@@ -3874,7 +3862,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
@@ -3883,7 +3871,7 @@
         <v>9</v>
       </c>
       <c r="D117" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E117">
         <v>2.5</v>
@@ -3914,10 +3902,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B119" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C119" t="s">
         <v>77</v>
@@ -3929,7 +3917,7 @@
         <v>7</v>
       </c>
       <c r="G119" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>